<commit_message>
Remove requirement for main contributor (creator)
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example_batch_ingest/missing_required_field.xlsx
+++ b/spec/fixtures/dropbox/example_batch_ingest/missing_required_field.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Missing Required Field</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>content/0276 med.mp4</t>
-  </si>
-  <si>
-    <t>Test Batch - File 2 with space</t>
   </si>
   <si>
     <t>content/tone loc.wav</t>
@@ -100,7 +97,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -143,21 +140,21 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="thin"/>
+      <right style="hair"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thick"/>
       <top/>
@@ -166,67 +163,67 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -234,33 +231,34 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5395348837209"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.506976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.493023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.0046511627907"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.493023255814"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.4976744186047"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.537037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.4925925925926"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.4925925925926"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.4962962962963"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.8232558139535"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="10.493023255814"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.9953488372093"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.8325581395349"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="10.493023255814"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.8222222222222"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="10.8333333333333"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="10.8333333333333"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="10.4925925925926"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.837037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="10.4925925925926"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -270,11 +268,11 @@
       <c r="M1" s="0"/>
       <c r="N1" s="0"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -326,7 +324,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>20</v>
       </c>
@@ -343,10 +341,7 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="s">
-        <v>24</v>
-      </c>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G4" s="0" t="n">
         <v>2014</v>
       </c>
@@ -357,14 +352,14 @@
         <v>22</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="5"/>
+    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>